<commit_message>
Fix in AP Connection Routines
Change-Id: Ie8a3dce308f0d3e73f20738f9364f34d15ac5544
Signed-off-by: Andrey Shamis <lolnik@gmail.com>
</commit_message>
<xml_diff>
--- a/SLS Rates.xlsx
+++ b/SLS Rates.xlsx
@@ -822,11 +822,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="127304192"/>
-        <c:axId val="122001600"/>
+        <c:axId val="88620032"/>
+        <c:axId val="64705600"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="127304192"/>
+        <c:axId val="88620032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -836,7 +836,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="122001600"/>
+        <c:crossAx val="64705600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -844,7 +844,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="122001600"/>
+        <c:axId val="64705600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -874,7 +874,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="127304192"/>
+        <c:crossAx val="88620032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -897,20 +897,1715 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="144"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="44"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-61</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$3:$E$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>300</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-62</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$4:$E$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>270</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-63</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$5:$E$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$6</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-64</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$6:$E$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-65</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$7:$E$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>270</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-66</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$8:$E$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>240</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="6"/>
+          <c:order val="6"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-67</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$9:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="7"/>
+          <c:order val="7"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$10</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-68</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$10:$E$10</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="8"/>
+          <c:order val="8"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-69</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$11:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>240</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="9"/>
+          <c:order val="9"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-70</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$12:$E$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>180</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="10"/>
+          <c:order val="10"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-71</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$13:$E$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="11"/>
+          <c:order val="11"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-72</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$14:$E$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="12"/>
+          <c:order val="12"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-73</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$15:$E$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>180</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>120</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="13"/>
+          <c:order val="13"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$16</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-74</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$16:$E$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="14"/>
+          <c:order val="14"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$17</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-75</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$17:$E$17</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="15"/>
+          <c:order val="15"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-76</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$18:$E$18</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="16"/>
+          <c:order val="16"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-77</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$19:$E$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="17"/>
+          <c:order val="17"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-78</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$20:$E$20</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>60</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="18"/>
+          <c:order val="18"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-79</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$21:$E$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="19"/>
+          <c:order val="19"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-80</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$22:$E$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="20"/>
+          <c:order val="20"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-81</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$23:$E$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="21"/>
+          <c:order val="21"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Лист1!$A$24</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>-82</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Лист1!$B$1:$E$2</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="4"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>20MHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>40MHz</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>2.4GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5GHz</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Лист1!$B$24:$E$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="38596096"/>
+        <c:axId val="58319424"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="38596096"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="58319424"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="58319424"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="38596096"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>409574</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>100011</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -924,6 +2619,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>571499</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Диаграмма 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1222,7 +2947,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E24"/>
+      <selection activeCell="E24" sqref="A1:E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>